<commit_message>
Update sample data for firebase.
</commit_message>
<xml_diff>
--- a/sample_data/data_structure.xlsx
+++ b/sample_data/data_structure.xlsx
@@ -9,23 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" tabRatio="859" xr2:uid="{C4815C0D-18B8-4187-B121-7EDB224FE5ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" tabRatio="859" firstSheet="6" activeTab="6" xr2:uid="{C4815C0D-18B8-4187-B121-7EDB224FE5ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="(done) EduYears" sheetId="10" r:id="rId1"/>
-    <sheet name="(done) Subjects" sheetId="6" r:id="rId2"/>
-    <sheet name="(done) Tutors" sheetId="7" r:id="rId3"/>
-    <sheet name="(done) Tutor Students" sheetId="9" r:id="rId4"/>
-    <sheet name="(done) Tutor Subjects" sheetId="2" r:id="rId5"/>
-    <sheet name="(done) Students" sheetId="14" r:id="rId6"/>
-    <sheet name="(done) Student Subjects" sheetId="8" r:id="rId7"/>
-    <sheet name="(KIV) Notes" sheetId="1" r:id="rId8"/>
-    <sheet name="(done) Ask Teacher" sheetId="5" r:id="rId9"/>
-    <sheet name="(done) Bookmark" sheetId="4" r:id="rId10"/>
-    <sheet name="(done) Report" sheetId="3" r:id="rId11"/>
-    <sheet name="(done) Country" sheetId="13" r:id="rId12"/>
-    <sheet name="(done) State" sheetId="12" r:id="rId13"/>
-    <sheet name="(done) District" sheetId="11" r:id="rId14"/>
+    <sheet name="(done-u) EduYears" sheetId="10" r:id="rId1"/>
+    <sheet name="(done-u) Subjects" sheetId="6" r:id="rId2"/>
+    <sheet name="(done-u) Tutors" sheetId="7" r:id="rId3"/>
+    <sheet name="(done-u) Tutor Students" sheetId="9" r:id="rId4"/>
+    <sheet name="(done-u) Tutor Subjects" sheetId="2" r:id="rId5"/>
+    <sheet name="(done-u) Students" sheetId="14" r:id="rId6"/>
+    <sheet name="(done-u) Student Subjects" sheetId="8" r:id="rId7"/>
+    <sheet name="(KIV-u) Notes" sheetId="1" r:id="rId8"/>
+    <sheet name="(done-u) Ask Teacher" sheetId="5" r:id="rId9"/>
+    <sheet name="(done-u) Bookmark" sheetId="4" r:id="rId10"/>
+    <sheet name="(done-u) Report" sheetId="3" r:id="rId11"/>
+    <sheet name="(done-u) Country" sheetId="13" r:id="rId12"/>
+    <sheet name="(done-u) State" sheetId="12" r:id="rId13"/>
+    <sheet name="(done-u) District" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="102">
   <si>
     <t>edu_years</t>
   </si>
@@ -1039,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C147B5A-2DD2-446F-B1AC-177358A068F0}">
   <dimension ref="B2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1339,7 +1339,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="54">
-        <f>'(done) Students'!D2</f>
+        <f>'(done-u) Students'!D2</f>
         <v>1</v>
       </c>
       <c r="G4" s="54"/>
@@ -1360,7 +1360,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="54" t="str">
-        <f>'(done) Students'!D3</f>
+        <f>'(done-u) Students'!D3</f>
         <v>Ahmad Yusoff</v>
       </c>
       <c r="G5" s="31" t="s">
@@ -1383,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="17">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="I6" s="31" t="s">
@@ -1399,11 +1399,11 @@
       <c r="A7"/>
       <c r="B7" s="38"/>
       <c r="I7" s="17" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="J7" s="58">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="L7" s="38"/>
@@ -1415,11 +1415,11 @@
       <c r="A8" s="10"/>
       <c r="B8" s="38"/>
       <c r="I8" s="17" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="J8" s="58" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="L8" s="38"/>
@@ -1431,11 +1431,11 @@
       <c r="A9" s="10"/>
       <c r="B9" s="38"/>
       <c r="I9" s="17" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="J9" s="58" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="K9" s="15" t="s">
@@ -1460,14 +1460,14 @@
         <v>13</v>
       </c>
       <c r="L10" s="44">
-        <f>'(KIV) Notes'!L12</f>
+        <f>'(KIV-u) Notes'!L12</f>
         <v>1</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="57">
-        <f>'(KIV) Notes'!L12</f>
+        <f>'(KIV-u) Notes'!L12</f>
         <v>1</v>
       </c>
       <c r="O10" s="57"/>
@@ -1490,7 +1490,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="57" t="str">
-        <f>'(KIV) Notes'!L13</f>
+        <f>'(KIV-u) Notes'!L13</f>
         <v>Function</v>
       </c>
       <c r="O11" s="15" t="s">
@@ -1512,11 +1512,11 @@
       <c r="K12" s="16"/>
       <c r="L12" s="44"/>
       <c r="O12" s="14" t="str">
-        <f>'(KIV) Notes'!O15</f>
+        <f>'(KIV-u) Notes'!O15</f>
         <v>subchapter_id</v>
       </c>
       <c r="P12" s="26">
-        <f>'(KIV) Notes'!P15</f>
+        <f>'(KIV-u) Notes'!P15</f>
         <v>1</v>
       </c>
       <c r="Q12" s="15" t="s">
@@ -1545,11 +1545,11 @@
       <c r="O13" s="16"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="14" t="str">
-        <f>'(KIV) Notes'!O15</f>
+        <f>'(KIV-u) Notes'!O15</f>
         <v>subchapter_id</v>
       </c>
       <c r="R13" s="54">
-        <f>'(KIV) Notes'!P15</f>
+        <f>'(KIV-u) Notes'!P15</f>
         <v>1</v>
       </c>
       <c r="S13" s="2"/>
@@ -1569,11 +1569,11 @@
       <c r="O14" s="16"/>
       <c r="P14" s="26"/>
       <c r="Q14" s="14" t="str">
-        <f>'(KIV) Notes'!O16</f>
+        <f>'(KIV-u) Notes'!O16</f>
         <v>subchapter_name</v>
       </c>
       <c r="R14" s="54" t="str">
-        <f>'(KIV) Notes'!P16</f>
+        <f>'(KIV-u) Notes'!P16</f>
         <v>Relation</v>
       </c>
       <c r="S14" s="25" t="s">
@@ -1853,7 +1853,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="54">
-        <f>'(done) Students'!D2</f>
+        <f>'(done-u) Students'!D2</f>
         <v>1</v>
       </c>
       <c r="G4" s="54"/>
@@ -1873,7 +1873,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="54" t="str">
-        <f>'(done) Students'!D3</f>
+        <f>'(done-u) Students'!D3</f>
         <v>Ahmad Yusoff</v>
       </c>
       <c r="G5" s="31" t="s">
@@ -1895,7 +1895,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="17">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="I6" s="31" t="s">
@@ -1910,11 +1910,11 @@
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="38"/>
       <c r="I7" s="17" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="J7" s="58">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="L7" s="38"/>
@@ -1926,11 +1926,11 @@
       <c r="A8" s="10"/>
       <c r="B8" s="38"/>
       <c r="I8" s="17" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="J8" s="58" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="L8" s="38"/>
@@ -1942,11 +1942,11 @@
       <c r="A9" s="10"/>
       <c r="B9" s="38"/>
       <c r="I9" s="17" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="J9" s="58" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="K9" s="15" t="s">
@@ -1971,14 +1971,14 @@
         <v>13</v>
       </c>
       <c r="L10" s="44">
-        <f>'(KIV) Notes'!L12</f>
+        <f>'(KIV-u) Notes'!L12</f>
         <v>1</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="57">
-        <f>'(KIV) Notes'!L12</f>
+        <f>'(KIV-u) Notes'!L12</f>
         <v>1</v>
       </c>
       <c r="O10" s="57"/>
@@ -2001,7 +2001,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="57" t="str">
-        <f>'(KIV) Notes'!L13</f>
+        <f>'(KIV-u) Notes'!L13</f>
         <v>Function</v>
       </c>
       <c r="O11" s="15" t="s">
@@ -2023,11 +2023,11 @@
       <c r="K12" s="16"/>
       <c r="L12" s="44"/>
       <c r="O12" s="14" t="str">
-        <f>'(KIV) Notes'!O15</f>
+        <f>'(KIV-u) Notes'!O15</f>
         <v>subchapter_id</v>
       </c>
       <c r="P12" s="26">
-        <f>'(KIV) Notes'!P15</f>
+        <f>'(KIV-u) Notes'!P15</f>
         <v>1</v>
       </c>
       <c r="Q12" s="15" t="s">
@@ -2056,11 +2056,11 @@
       <c r="O13" s="16"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="14" t="str">
-        <f>'(KIV) Notes'!O15</f>
+        <f>'(KIV-u) Notes'!O15</f>
         <v>subchapter_id</v>
       </c>
       <c r="R13" s="54">
-        <f>'(KIV) Notes'!P15</f>
+        <f>'(KIV-u) Notes'!P15</f>
         <v>1</v>
       </c>
       <c r="S13" s="2"/>
@@ -2080,11 +2080,11 @@
       <c r="O14" s="16"/>
       <c r="P14" s="26"/>
       <c r="Q14" s="14" t="str">
-        <f>'(KIV) Notes'!O16</f>
+        <f>'(KIV-u) Notes'!O16</f>
         <v>subchapter_name</v>
       </c>
       <c r="R14" s="54" t="str">
-        <f>'(KIV) Notes'!P16</f>
+        <f>'(KIV-u) Notes'!P16</f>
         <v>Relation</v>
       </c>
       <c r="S14" s="25" t="s">
@@ -2739,238 +2739,263 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F320FA-8D02-4E4A-A0E3-D73C230F4A3F}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15" t="s">
+      <c r="D1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="27"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
-      <c r="B3" s="17" t="str">
-        <f>'(done) EduYears'!D15</f>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="str">
+        <f>'(done-u) EduYears'!D15</f>
         <v>edu_year_id</v>
       </c>
-      <c r="C3" s="30">
-        <f>'(done) EduYears'!E15</f>
+      <c r="D3" s="30">
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="E3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="17" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="26">
-        <v>1</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="26">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H4" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="H5" s="57" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="H6" s="57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="I7" s="26"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
-      <c r="E8" s="26">
+      <c r="D8" s="16"/>
+      <c r="F8" s="26">
         <v>2</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="56">
+      <c r="H8" s="56">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17" t="s">
+      <c r="D9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="H9" s="57" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17" t="s">
+      <c r="D10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="H10" s="57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="16"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
-      <c r="E12" s="26">
+      <c r="D12" s="16"/>
+      <c r="F12" s="26">
         <v>3</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="56">
+      <c r="H12" s="56">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17" t="s">
+      <c r="D13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="57" t="s">
+      <c r="H13" s="57" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17" t="s">
+      <c r="D14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="H14" s="57" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
-      <c r="E16" s="26">
+      <c r="D16" s="16"/>
+      <c r="F16" s="26">
         <v>4</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="G16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="56">
+      <c r="H16" s="56">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17" t="s">
+      <c r="D17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="57" t="s">
+      <c r="H17" s="57" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17" t="s">
+      <c r="D18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="57" t="s">
+      <c r="H18" s="57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="F19" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2982,7 +3007,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,7 +3033,9 @@
       <c r="H2" s="44"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
+      <c r="B3" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="15" t="s">
         <v>0</v>
       </c>
@@ -3021,11 +3048,11 @@
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="19"/>
       <c r="C4" s="17" t="str">
-        <f>'(done) EduYears'!D15</f>
+        <f>'(done-u) EduYears'!D15</f>
         <v>edu_year_id</v>
       </c>
       <c r="D4" s="59">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="E4" s="30"/>
@@ -3036,11 +3063,11 @@
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="19"/>
       <c r="C5" s="17" t="str">
-        <f>'(done) EduYears'!D16</f>
+        <f>'(done-u) EduYears'!D16</f>
         <v>edu_year_title_my</v>
       </c>
       <c r="D5" s="59" t="str">
-        <f>'(done) EduYears'!E16</f>
+        <f>'(done-u) EduYears'!E16</f>
         <v>Tingkatan 4</v>
       </c>
       <c r="E5" s="30"/>
@@ -3052,11 +3079,11 @@
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="19"/>
       <c r="C6" s="17" t="str">
-        <f>'(done) EduYears'!D17</f>
+        <f>'(done-u) EduYears'!D17</f>
         <v>edu_year_title_en</v>
       </c>
       <c r="D6" s="59" t="str">
-        <f>'(done) EduYears'!E17</f>
+        <f>'(done-u) EduYears'!E17</f>
         <v>Form 4</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -3194,11 +3221,11 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="str">
-        <f>'(done) Tutors'!G8</f>
+        <f>'(done-u) Tutors'!G8</f>
         <v>tutor_id</v>
       </c>
       <c r="B2" s="26">
-        <f>'(done) Tutors'!H8</f>
+        <f>'(done-u) Tutors'!H8</f>
         <v>1</v>
       </c>
       <c r="C2" s="42" t="s">
@@ -3207,11 +3234,11 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="str">
-        <f>'(done) Tutors'!G8</f>
+        <f>'(done-u) Tutors'!G8</f>
         <v>tutor_id</v>
       </c>
       <c r="D3" s="26">
-        <f>'(done) Tutors'!H8</f>
+        <f>'(done-u) Tutors'!H8</f>
         <v>1</v>
       </c>
       <c r="E3" s="26"/>
@@ -3219,11 +3246,11 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="str">
-        <f>'(done) Tutors'!G9</f>
+        <f>'(done-u) Tutors'!G9</f>
         <v>tutor_name</v>
       </c>
       <c r="D4" s="26" t="str">
-        <f>'(done) Tutors'!H9</f>
+        <f>'(done-u) Tutors'!H9</f>
         <v>Cg Imran</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -3237,7 +3264,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="18">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="G5" s="12" t="s">
@@ -3248,33 +3275,33 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G6" s="14" t="str">
-        <f>'(done) EduYears'!D3</f>
+        <f>'(done-u) EduYears'!D3</f>
         <v>edu_year_id</v>
       </c>
       <c r="H6" s="40">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G7" s="14" t="str">
-        <f>'(done) EduYears'!D4</f>
+        <f>'(done-u) EduYears'!D4</f>
         <v>edu_year_title_my</v>
       </c>
       <c r="H7" s="40" t="str">
-        <f>'(done) EduYears'!E16</f>
+        <f>'(done-u) EduYears'!E16</f>
         <v>Tingkatan 4</v>
       </c>
       <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G8" s="14" t="str">
-        <f>'(done) EduYears'!D5</f>
+        <f>'(done-u) EduYears'!D5</f>
         <v>edu_year_title_en</v>
       </c>
       <c r="H8" s="40" t="str">
-        <f>'(done) EduYears'!E17</f>
+        <f>'(done-u) EduYears'!E17</f>
         <v>Form 4</v>
       </c>
       <c r="I8" s="44" t="s">
@@ -3291,21 +3318,21 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J10" s="14" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="K10" s="26">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J11" s="14" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="K11" s="26" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="O11" s="26"/>
@@ -3313,11 +3340,11 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J12" s="14" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="K12" s="26" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="L12" s="39" t="s">
@@ -3335,21 +3362,21 @@
         <v>1</v>
       </c>
       <c r="M13" s="14" t="str">
-        <f>'(done) Students'!C2</f>
+        <f>'(done-u) Students'!C2</f>
         <v>student_id</v>
       </c>
       <c r="N13" s="26">
-        <f>'(done) Students'!D2</f>
+        <f>'(done-u) Students'!D2</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M14" s="14" t="str">
-        <f>'(done) Students'!C3</f>
+        <f>'(done-u) Students'!C3</f>
         <v>student_name</v>
       </c>
       <c r="N14" s="26" t="str">
-        <f>'(done) Students'!D3</f>
+        <f>'(done-u) Students'!D3</f>
         <v>Ahmad Yusoff</v>
       </c>
       <c r="O14" s="26"/>
@@ -3362,21 +3389,21 @@
         <v>2</v>
       </c>
       <c r="M16" s="14" t="str">
-        <f>'(done) Students'!C5</f>
+        <f>'(done-u) Students'!C5</f>
         <v>student_id</v>
       </c>
       <c r="N16" s="26">
-        <f>'(done) Students'!D5</f>
+        <f>'(done-u) Students'!D5</f>
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="12:14" x14ac:dyDescent="0.25">
       <c r="M17" s="14" t="str">
-        <f>'(done) Students'!C6</f>
+        <f>'(done-u) Students'!C6</f>
         <v>student_name</v>
       </c>
       <c r="N17" s="26" t="str">
-        <f>'(done) Students'!D6</f>
+        <f>'(done-u) Students'!D6</f>
         <v>Muhammad Naim</v>
       </c>
     </row>
@@ -3385,21 +3412,21 @@
         <v>3</v>
       </c>
       <c r="M19" s="14" t="str">
-        <f>'(done) Students'!C8</f>
+        <f>'(done-u) Students'!C8</f>
         <v>student_id</v>
       </c>
       <c r="N19" s="26">
-        <f>'(done) Students'!D8</f>
+        <f>'(done-u) Students'!D8</f>
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="12:14" x14ac:dyDescent="0.25">
       <c r="M20" s="14" t="str">
-        <f>'(done) Students'!C9</f>
+        <f>'(done-u) Students'!C9</f>
         <v>student_name</v>
       </c>
       <c r="N20" s="26" t="str">
-        <f>'(done) Students'!D9</f>
+        <f>'(done-u) Students'!D9</f>
         <v>Muhammad Hassan Husni</v>
       </c>
     </row>
@@ -3449,7 +3476,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="30">
-        <f>'(done) Tutors'!H8</f>
+        <f>'(done-u) Tutors'!H8</f>
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
@@ -3469,11 +3496,11 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="str">
-        <f>'(done) Tutors'!G8</f>
+        <f>'(done-u) Tutors'!G8</f>
         <v>tutor_id</v>
       </c>
       <c r="D4" s="56">
-        <f>'(done) Tutors'!H8</f>
+        <f>'(done-u) Tutors'!H8</f>
         <v>1</v>
       </c>
       <c r="E4" s="26"/>
@@ -3490,11 +3517,11 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="str">
-        <f>'(done) Tutors'!G9</f>
+        <f>'(done-u) Tutors'!G9</f>
         <v>tutor_name</v>
       </c>
       <c r="D5" s="56" t="str">
-        <f>'(done) Tutors'!H9</f>
+        <f>'(done-u) Tutors'!H9</f>
         <v>Cg Imran</v>
       </c>
       <c r="E5" s="15" t="s">
@@ -3513,19 +3540,19 @@
       <c r="C6" s="28"/>
       <c r="D6" s="63"/>
       <c r="E6" s="17" t="str">
-        <f>'(done) EduYears'!D15</f>
+        <f>'(done-u) EduYears'!D15</f>
         <v>edu_year_id</v>
       </c>
       <c r="F6" s="27">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="G6" s="17" t="str">
-        <f>'(done) EduYears'!D15</f>
+        <f>'(done-u) EduYears'!D15</f>
         <v>edu_year_id</v>
       </c>
       <c r="H6" s="58">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="I6" s="27"/>
@@ -3539,11 +3566,11 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="17" t="str">
-        <f>'(done) EduYears'!D16</f>
+        <f>'(done-u) EduYears'!D16</f>
         <v>edu_year_title_my</v>
       </c>
       <c r="H7" s="58" t="str">
-        <f>'(done) EduYears'!E16</f>
+        <f>'(done-u) EduYears'!E16</f>
         <v>Tingkatan 4</v>
       </c>
       <c r="I7" s="27"/>
@@ -3558,11 +3585,11 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="17" t="str">
-        <f>'(done) EduYears'!D17</f>
+        <f>'(done-u) EduYears'!D17</f>
         <v>edu_year_title_en</v>
       </c>
       <c r="H8" s="58" t="str">
-        <f>'(done) EduYears'!E17</f>
+        <f>'(done-u) EduYears'!E17</f>
         <v>Form 4</v>
       </c>
       <c r="I8" s="4" t="str">
@@ -3570,7 +3597,7 @@
         <v>subjects</v>
       </c>
       <c r="K8" s="4" t="str">
-        <f>'(done) Subjects'!F3</f>
+        <f>'(done-u) Subjects'!G3</f>
         <v>subjects</v>
       </c>
     </row>
@@ -3591,11 +3618,11 @@
         <v>1</v>
       </c>
       <c r="K9" s="6" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="L9" s="56">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="M9" s="26"/>
@@ -3613,11 +3640,11 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="6" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="L10" s="56" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="M10" s="26"/>
@@ -3626,11 +3653,11 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K11" s="6" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="L11" s="56" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="M11" s="26"/>
@@ -3646,32 +3673,32 @@
         <v>2</v>
       </c>
       <c r="K13" s="6" t="str">
-        <f>'(done) Subjects'!F8</f>
+        <f>'(done-u) Subjects'!G8</f>
         <v>subject_id</v>
       </c>
       <c r="L13" s="56">
-        <f>'(done) Subjects'!G8</f>
+        <f>'(done-u) Subjects'!H8</f>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J14" s="2"/>
       <c r="K14" s="6" t="str">
-        <f>'(done) Subjects'!F9</f>
+        <f>'(done-u) Subjects'!G9</f>
         <v>subject_nam_my</v>
       </c>
       <c r="L14" s="56" t="str">
-        <f>'(done) Subjects'!G9</f>
+        <f>'(done-u) Subjects'!H9</f>
         <v>Matematik</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K15" s="6" t="str">
-        <f>'(done) Subjects'!F10</f>
+        <f>'(done-u) Subjects'!G10</f>
         <v>subject_nam_en</v>
       </c>
       <c r="L15" s="56" t="str">
-        <f>'(done) Subjects'!G10</f>
+        <f>'(done-u) Subjects'!H10</f>
         <v>Mathematics</v>
       </c>
     </row>
@@ -3684,31 +3711,31 @@
         <v>3</v>
       </c>
       <c r="K17" s="6" t="str">
-        <f>'(done) Subjects'!F12</f>
+        <f>'(done-u) Subjects'!G12</f>
         <v>subject_id</v>
       </c>
       <c r="L17" s="56">
-        <f>'(done) Subjects'!G12</f>
+        <f>'(done-u) Subjects'!H12</f>
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K18" s="6" t="str">
-        <f>'(done) Subjects'!F13</f>
+        <f>'(done-u) Subjects'!G13</f>
         <v>subject_nam_my</v>
       </c>
       <c r="L18" s="56" t="str">
-        <f>'(done) Subjects'!G13</f>
+        <f>'(done-u) Subjects'!H13</f>
         <v>Fizik</v>
       </c>
     </row>
     <row r="19" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K19" s="6" t="str">
-        <f>'(done) Subjects'!F14</f>
+        <f>'(done-u) Subjects'!G14</f>
         <v>subject_nam_en</v>
       </c>
       <c r="L19" s="56" t="str">
-        <f>'(done) Subjects'!G14</f>
+        <f>'(done-u) Subjects'!H14</f>
         <v>Physics</v>
       </c>
     </row>
@@ -3832,7 +3859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D380EC72-AF6F-4A6B-A8D8-7C48F6E5F755}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -3890,11 +3917,11 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="17" t="str">
-        <f>'(done) EduYears'!D15</f>
+        <f>'(done-u) EduYears'!D15</f>
         <v>edu_year_id</v>
       </c>
       <c r="E4" s="58">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="H4" s="46"/>
@@ -3907,11 +3934,11 @@
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="17" t="str">
-        <f>'(done) EduYears'!D16</f>
+        <f>'(done-u) EduYears'!D16</f>
         <v>edu_year_title_my</v>
       </c>
       <c r="E5" s="58" t="str">
-        <f>'(done) EduYears'!E16</f>
+        <f>'(done-u) EduYears'!E16</f>
         <v>Tingkatan 4</v>
       </c>
     </row>
@@ -3919,11 +3946,11 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="17" t="str">
-        <f>'(done) EduYears'!D17</f>
+        <f>'(done-u) EduYears'!D17</f>
         <v>edu_year_title_en</v>
       </c>
       <c r="E6" s="58" t="str">
-        <f>'(done) EduYears'!E17</f>
+        <f>'(done-u) EduYears'!E17</f>
         <v>Form 4</v>
       </c>
       <c r="F6" s="42" t="s">
@@ -3942,7 +3969,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="65">
-        <f>'(done) Students'!D2</f>
+        <f>'(done-u) Students'!D2</f>
         <v>1</v>
       </c>
       <c r="H7" s="2"/>
@@ -3959,7 +3986,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="65" t="str">
-        <f>'(done) Students'!D3</f>
+        <f>'(done-u) Students'!D3</f>
         <v>Ahmad Yusoff</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -3980,19 +4007,19 @@
       <c r="F9" s="28"/>
       <c r="G9" s="63"/>
       <c r="H9" s="6" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="I9" s="26">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="J9" s="6" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="K9" s="66">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="M9" s="11"/>
@@ -4008,11 +4035,11 @@
       <c r="H10" s="6"/>
       <c r="I10" s="26"/>
       <c r="J10" s="6" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="K10" s="66" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="L10" s="26"/>
@@ -4025,11 +4052,11 @@
       <c r="H11" s="6"/>
       <c r="I11" s="26"/>
       <c r="J11" s="6" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="K11" s="66" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="L11" s="26"/>
@@ -4043,69 +4070,69 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I13" s="26">
-        <f>'(done) Subjects'!G8</f>
+        <f>'(done-u) Subjects'!H8</f>
         <v>2</v>
       </c>
       <c r="J13" s="6" t="str">
-        <f>'(done) Subjects'!F8</f>
+        <f>'(done-u) Subjects'!G8</f>
         <v>subject_id</v>
       </c>
       <c r="K13" s="66">
-        <f>'(done) Subjects'!G8</f>
+        <f>'(done-u) Subjects'!H8</f>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J14" s="6" t="str">
-        <f>'(done) Subjects'!F9</f>
+        <f>'(done-u) Subjects'!G9</f>
         <v>subject_nam_my</v>
       </c>
       <c r="K14" s="66" t="str">
-        <f>'(done) Subjects'!G9</f>
+        <f>'(done-u) Subjects'!H9</f>
         <v>Matematik</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J15" s="6" t="str">
-        <f>'(done) Subjects'!F10</f>
+        <f>'(done-u) Subjects'!G10</f>
         <v>subject_nam_en</v>
       </c>
       <c r="K15" s="66" t="str">
-        <f>'(done) Subjects'!G10</f>
+        <f>'(done-u) Subjects'!H10</f>
         <v>Mathematics</v>
       </c>
     </row>
     <row r="17" spans="9:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I17" s="26">
-        <f>'(done) Subjects'!G12</f>
+        <f>'(done-u) Subjects'!H12</f>
         <v>3</v>
       </c>
       <c r="J17" s="6" t="str">
-        <f>'(done) Subjects'!F12</f>
+        <f>'(done-u) Subjects'!G12</f>
         <v>subject_id</v>
       </c>
       <c r="K17" s="66">
-        <f>'(done) Subjects'!G12</f>
+        <f>'(done-u) Subjects'!H12</f>
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="9:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J18" s="6" t="str">
-        <f>'(done) Subjects'!F13</f>
+        <f>'(done-u) Subjects'!G13</f>
         <v>subject_nam_my</v>
       </c>
       <c r="K18" s="66" t="str">
-        <f>'(done) Subjects'!G13</f>
+        <f>'(done-u) Subjects'!H13</f>
         <v>Fizik</v>
       </c>
     </row>
     <row r="19" spans="9:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J19" s="6" t="str">
-        <f>'(done) Subjects'!F14</f>
+        <f>'(done-u) Subjects'!G14</f>
         <v>subject_nam_en</v>
       </c>
       <c r="K19" s="66" t="str">
-        <f>'(done) Subjects'!G14</f>
+        <f>'(done-u) Subjects'!H14</f>
         <v>Physics</v>
       </c>
     </row>
@@ -4118,8 +4145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C0D756-173B-480F-A1D2-BC692AD12C29}">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="A7:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,11 +4206,11 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="str">
-        <f>'(done) EduYears'!D15</f>
+        <f>'(done-u) EduYears'!D15</f>
         <v>edu_year_id</v>
       </c>
       <c r="D4" s="58">
-        <f>'(done) EduYears'!E15</f>
+        <f>'(done-u) EduYears'!E15</f>
         <v>10</v>
       </c>
       <c r="E4" s="29"/>
@@ -4201,11 +4228,11 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="str">
-        <f>'(done) EduYears'!D16</f>
+        <f>'(done-u) EduYears'!D16</f>
         <v>edu_year_title_my</v>
       </c>
       <c r="D5" s="58" t="str">
-        <f>'(done) EduYears'!E16</f>
+        <f>'(done-u) EduYears'!E16</f>
         <v>Tingkatan 4</v>
       </c>
       <c r="K5" s="16"/>
@@ -4218,11 +4245,11 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="17" t="str">
-        <f>'(done) EduYears'!D17</f>
+        <f>'(done-u) EduYears'!D17</f>
         <v>edu_year_title_en</v>
       </c>
       <c r="D6" s="58" t="str">
-        <f>'(done) EduYears'!E17</f>
+        <f>'(done-u) EduYears'!E17</f>
         <v>Form 4</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -4244,11 +4271,11 @@
       <c r="C7" s="19"/>
       <c r="D7" s="27"/>
       <c r="E7" s="17" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="F7" s="44">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="G7" s="31" t="s">
@@ -4268,11 +4295,11 @@
       <c r="D8" s="27"/>
       <c r="E8" s="17"/>
       <c r="G8" s="17" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="H8" s="58">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="I8" s="58"/>
@@ -4286,11 +4313,11 @@
       <c r="C9" s="19"/>
       <c r="D9" s="27"/>
       <c r="G9" s="17" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="H9" s="58" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="I9" s="58"/>
@@ -4305,11 +4332,11 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="G10" s="17" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="H10" s="58" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="I10" s="15" t="s">
@@ -4574,7 +4601,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V24" sqref="A1:V24"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4660,7 +4687,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="54">
-        <f>'(done) Students'!D2</f>
+        <f>'(done-u) Students'!D2</f>
         <v>1</v>
       </c>
       <c r="G4" s="54"/>
@@ -4678,7 +4705,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="54" t="str">
-        <f>'(done) Students'!D3</f>
+        <f>'(done-u) Students'!D3</f>
         <v>Ahmad Yusoff</v>
       </c>
       <c r="G5" s="31" t="s">
@@ -4698,7 +4725,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="17">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="I6" s="31" t="s">
@@ -4710,11 +4737,11 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I7" s="17" t="str">
-        <f>'(done) Subjects'!F4</f>
+        <f>'(done-u) Subjects'!G4</f>
         <v>subject_id</v>
       </c>
       <c r="J7" s="58">
-        <f>'(done) Subjects'!G4</f>
+        <f>'(done-u) Subjects'!H4</f>
         <v>1</v>
       </c>
       <c r="Q7" s="16"/>
@@ -4723,11 +4750,11 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="I8" s="17" t="str">
-        <f>'(done) Subjects'!F5</f>
+        <f>'(done-u) Subjects'!G5</f>
         <v>subject_nam_my</v>
       </c>
       <c r="J8" s="58" t="str">
-        <f>'(done) Subjects'!G5</f>
+        <f>'(done-u) Subjects'!H5</f>
         <v>Matematik Tambahan</v>
       </c>
       <c r="Q8" s="15"/>
@@ -4736,11 +4763,11 @@
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="I9" s="17" t="str">
-        <f>'(done) Subjects'!F6</f>
+        <f>'(done-u) Subjects'!G6</f>
         <v>subject_nam_en</v>
       </c>
       <c r="J9" s="58" t="str">
-        <f>'(done) Subjects'!G6</f>
+        <f>'(done-u) Subjects'!H6</f>
         <v>Additional Mathematics</v>
       </c>
       <c r="K9" s="15" t="s">
@@ -4763,14 +4790,14 @@
         <v>13</v>
       </c>
       <c r="L10" s="44">
-        <f>'(KIV) Notes'!L12</f>
+        <f>'(KIV-u) Notes'!L12</f>
         <v>1</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="57">
-        <f>'(KIV) Notes'!L12</f>
+        <f>'(KIV-u) Notes'!L12</f>
         <v>1</v>
       </c>
       <c r="O10" s="57"/>
@@ -4793,7 +4820,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="57" t="str">
-        <f>'(KIV) Notes'!L13</f>
+        <f>'(KIV-u) Notes'!L13</f>
         <v>Function</v>
       </c>
       <c r="O11" s="15" t="s">
@@ -4815,11 +4842,11 @@
       <c r="K12" s="16"/>
       <c r="L12" s="44"/>
       <c r="O12" s="14" t="str">
-        <f>'(KIV) Notes'!O15</f>
+        <f>'(KIV-u) Notes'!O15</f>
         <v>subchapter_id</v>
       </c>
       <c r="P12" s="26">
-        <f>'(KIV) Notes'!P15</f>
+        <f>'(KIV-u) Notes'!P15</f>
         <v>1</v>
       </c>
       <c r="Q12" s="15" t="s">
@@ -4848,11 +4875,11 @@
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
       <c r="Q13" s="14" t="str">
-        <f>'(KIV) Notes'!O15</f>
+        <f>'(KIV-u) Notes'!O15</f>
         <v>subchapter_id</v>
       </c>
       <c r="R13" s="54">
-        <f>'(KIV) Notes'!P15</f>
+        <f>'(KIV-u) Notes'!P15</f>
         <v>1</v>
       </c>
       <c r="S13" s="2"/>
@@ -4872,11 +4899,11 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
       <c r="Q14" s="14" t="str">
-        <f>'(KIV) Notes'!O16</f>
+        <f>'(KIV-u) Notes'!O16</f>
         <v>subchapter_name</v>
       </c>
       <c r="R14" s="54" t="str">
-        <f>'(KIV) Notes'!P16</f>
+        <f>'(KIV-u) Notes'!P16</f>
         <v>Relation</v>
       </c>
       <c r="S14" s="25" t="s">

</xml_diff>